<commit_message>
Add additional splitter with same produced example set for different amounts of training data up to N=50 ratings per user
</commit_message>
<xml_diff>
--- a/results/complete.xlsx
+++ b/results/complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helena Graf\git\cofirank\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{17D94DE5-20E5-428B-8D42-2A46671390E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49E2196-D6BE-4DFF-AA88-B28E7B6D5688}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D0323EC-577F-4570-A2FF-599DD2B299CE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>movielens_NDCG</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Optimizing for Regression yields better NDCG results than optimizing for NDCG (this is also the case in the paper)</t>
+  </si>
+  <si>
+    <t>movielens strong evaluation -&gt; not evalable with NDCG, leads to segmentation fault. Works with regression but I didn't do a complete eval because it is not comparable anyway (though the 1 result I did get seems to be superior to NDCG case)</t>
+  </si>
+  <si>
+    <t>also I am not entirely sure if I understood the procedure of the strong evaluation correcly</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -319,159 +325,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -783,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34026AD9-B8D9-4593-A5B7-758DCA8FE89C}">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,15 +1550,15 @@
         <v>16</v>
       </c>
       <c r="R22">
-        <f t="shared" ref="R22:R27" si="0">S13-R13</f>
+        <f t="shared" ref="R22:R26" si="0">S13-R13</f>
         <v>-1.7599999999999949E-2</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:S27" si="1">U13-T13</f>
+        <f t="shared" ref="S22:S26" si="1">U13-T13</f>
         <v>-4.1699999999999959E-2</v>
       </c>
       <c r="T22" s="1">
-        <f t="shared" ref="T22:T27" si="2">W13-V13</f>
+        <f t="shared" ref="T22:T23" si="2">W13-V13</f>
         <v>-7.1799999999999975E-2</v>
       </c>
     </row>
@@ -1883,6 +1736,16 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>